<commit_message>
update code from mac
</commit_message>
<xml_diff>
--- a/arrange_day_0/res.xlsx
+++ b/arrange_day_0/res.xlsx
@@ -8,22 +8,41 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yu_hsuan_chen/PycharmProjects/MEMDS/arrange_day_0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{F9D6AC55-6D98-CE45-B32F-4A61354FC4E5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{C7B541E2-B316-754F-8CE4-70DDE074DEA7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="res" sheetId="1" r:id="rId1"/>
-    <sheet name="cos" sheetId="2" r:id="rId2"/>
-    <sheet name="tfidf" sheetId="3" r:id="rId3"/>
-    <sheet name="tfpdf" sheetId="4" r:id="rId4"/>
+    <sheet name="compare" sheetId="5" r:id="rId1"/>
+    <sheet name="res" sheetId="1" r:id="rId2"/>
+    <sheet name="cos" sheetId="2" r:id="rId3"/>
+    <sheet name="tfidf" sheetId="3" r:id="rId4"/>
+    <sheet name="tfpdf" sheetId="4" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">compare!$A$1</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">compare!$A$2:$A$100</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">compare!$B$1</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">compare!$B$2:$B$100</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">compare!$C$1</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">compare!$C$2:$C$100</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">compare!$D$1</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">compare!$D$2:$D$100</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">compare!$B$1</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">compare!$B$2:$B$100</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">compare!$C$1</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">compare!$C$2:$C$100</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">compare!$D$1</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">compare!$D$2:$D$100</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">compare!$A$1</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">compare!$A$2:$A$100</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="7">
   <si>
     <t>accuracy</t>
   </si>
@@ -35,6 +54,18 @@
   </si>
   <si>
     <t>f1_score</t>
+  </si>
+  <si>
+    <t>cosine</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>tf-idf</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>tf-pdf</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -771,6 +802,2186 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
+              <c:f>compare!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>cosine</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>compare!$A$2:$A$100</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="99"/>
+                <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.14000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.24</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.27</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.28000000000000003</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.28999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.31</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.32</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.33</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.34</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.37</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.38</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.39</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.41</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.42</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.43</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.44</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.46</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.47</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.48</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.49</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.51</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.52</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.53</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.54</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.56000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.56999999999999995</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.57999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.59</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.61</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.63</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.64</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.66</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.67</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.68</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.69</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.71</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.72</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.73</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.74</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.76</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.77</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.78</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.79</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.81</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.82</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.84</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0.86</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0.87</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0.88</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0.89</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0.91</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0.92</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0.93</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0.94</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0.96</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0.97</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0.98</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0.99</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>compare!$B$2:$B$100</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="99"/>
+                <c:pt idx="0">
+                  <c:v>3.6572136990546997E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.6572136990546997E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.6572136990546997E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.6572136990546997E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.6572136990546997E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.6572136990546997E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.7192098596760823E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.7192098596760823E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.7347065278924155E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.7347065278924155E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.7347065278924155E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.7347065278924155E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.765699864325082E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.7811965325414159E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.7811965325414159E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.9062833425809598E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6.0476350948113718E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5.5417367220934648E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5.2666708612535501E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.10241305262225758</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.136476842543788</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.19740058484828349</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.21175831763480046</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.19233353100096384</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.26026173763323857</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.27004936069079538</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.25767952870722538</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.38817494391526863</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.48557450204415947</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.44132212821878902</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.43281530847555</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.43331597371757158</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.49182648813908819</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.49094694052225868</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.49693769953242622</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.56882727247349874</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.54167960314830543</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.58410664654443356</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.6009564748137397</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.59916752120347194</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.6161743239245604</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.60797963190633886</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.60252292247359451</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.59268094667808768</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.56887347269240196</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.56647695853118185</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.56205502514877514</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.53958087630401774</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.53705276072912522</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.52392673211542806</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.54912958719901139</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.52725918579099806</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.44705063588571803</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.44027491390555074</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.42524174014221838</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.42306953169497646</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.42193574484690388</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.37830959873628572</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.45219625041865069</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.44535956082089762</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.44117002492423446</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.43165324177962883</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.36088406782002624</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.29007392558131267</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.27069363867991125</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.27069363867991125</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.26932189656742828</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.26273821379769696</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.26136647168521421</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.25147366825458356</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.17957494222442316</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.17758333338328691</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.17758333338328691</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.17758333338328691</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.17419702440268059</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.17419702440268059</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.17419702440268059</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.17357715767402729</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.17130958397788212</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.17130958397788212</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>8.6974501734850218E-2</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>7.3257080610021771E-2</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>7.3257080610021771E-2</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>7.3257080610021771E-2</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>7.3257080610021771E-2</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>7.3257080610021771E-2</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>7.3257080610021771E-2</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>7.3257080610021771E-2</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>7.3257080610021771E-2</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>7.3257080610021771E-2</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>7.3257080610021771E-2</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>7.3257080610021771E-2</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>7.3257080610021771E-2</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>7.3257080610021771E-2</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>7.3257080610021771E-2</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>7.3257080610021771E-2</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>7.3257080610021771E-2</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>7.3257080610021771E-2</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>7.3257080610021771E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C681-B14E-88EB-832DC22AF12C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>compare!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>tf-idf</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>compare!$A$2:$A$100</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="99"/>
+                <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.14000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.24</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.27</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.28000000000000003</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.28999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.31</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.32</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.33</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.34</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.37</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.38</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.39</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.41</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.42</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.43</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.44</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.46</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.47</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.48</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.49</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.51</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.52</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.53</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.54</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.56000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.56999999999999995</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.57999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.59</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.61</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.63</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.64</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.66</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.67</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.68</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.69</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.71</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.72</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.73</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.74</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.76</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.77</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.78</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.79</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.81</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.82</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.84</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0.86</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0.87</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0.88</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0.89</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0.91</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0.92</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0.93</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0.94</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0.96</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0.97</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0.98</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0.99</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>compare!$C$2:$C$100</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="99"/>
+                <c:pt idx="0">
+                  <c:v>3.6572136990546997E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.6572136990546997E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.6727103672710336E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.6727103672710336E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.7037037037037E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.7394023921220443E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.7753833599176735E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.5344231070028513E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.16403752125440027</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.32895873009570953</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.3830870177211072</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.34881156399013036</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.39558102577346793</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.50608983329380175</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.5373553396289581</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.58127156729278673</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.66138575374700947</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.59158112835056398</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.65535281005058854</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.64164407837124737</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.64144613001441009</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.64680549119702069</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.62922387414536485</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.6204277110236186</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.63855246641545493</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.63518226044537562</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.61389547346821205</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.61300301474442809</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.60089482065526278</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.6154601278773586</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.60796463956345592</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.58454572179816844</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.5953468995449529</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.59178183715636112</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.57704260813141783</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.57733969666380036</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.56209994689421139</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.56529248656032638</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.56345509938285465</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.56156514980856342</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.48782727214192723</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.48289400097816326</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.48289400097816326</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.47319227106062189</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.47761299051539052</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.54561929469190751</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.54121753398762573</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.47690586554514841</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.47690586554514841</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.47690586554514841</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.4278396242205118</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.42976083766564521</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.42976083766564521</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.36172096015933053</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.35795881721283523</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.357076378036562</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.42700051904504033</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.36941871791762826</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.36941871791762826</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.29681720073779777</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.29340811927738053</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.28959438261922277</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.28959438261922277</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.28959438261922277</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.28959438261922277</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.28959438261922277</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.28614372699465407</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.28683385811956774</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.28683385811956774</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.28614372699465407</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.28614372699465407</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.2845940601730208</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.2845940601730208</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.2845940601730208</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.2845940601730208</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.28276756856130136</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.14656725535534879</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.14656725535534879</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.14656725535534879</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.14612102599345678</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.14612102599345678</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.14567479663156477</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0.27981025968466283</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.27981025968466283</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0.27912012855974921</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0.27887622679672741</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0.25575882791592508</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0.20133705920844222</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0.20158096097146397</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0.13123747522724488</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0.1969523706959381</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0.19605991197215411</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0.19605991197215411</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0.19605991197215411</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0.19605991197215411</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0.19561368261026213</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0.19561368261026213</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0.19492355148534846</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0.19492355148534846</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-C681-B14E-88EB-832DC22AF12C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>compare!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>tf-pdf</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>compare!$A$2:$A$100</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="99"/>
+                <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.14000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.24</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.27</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.28000000000000003</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.28999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.31</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.32</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.33</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.34</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.37</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.38</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.39</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.41</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.42</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.43</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.44</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.46</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.47</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.48</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.49</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.51</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.52</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.53</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.54</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.56000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.56999999999999995</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.57999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.59</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.61</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.63</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.64</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.66</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.67</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.68</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.69</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.71</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.72</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.73</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.74</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.76</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.77</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.78</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.79</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.81</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.82</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.84</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0.86</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0.87</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0.88</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0.89</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0.91</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0.92</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0.93</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0.94</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0.96</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0.97</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0.98</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0.99</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>compare!$D$2:$D$100</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="99"/>
+                <c:pt idx="0">
+                  <c:v>3.6623215394165111E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.7245341339515273E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.7245341339515273E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.7245341339515273E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.7245341339515273E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.7400524455592265E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.7400524455592265E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.7555707571669159E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.7555707571669159E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.8504541481396948E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.8504541481396948E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.8504541481396948E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.8504541481396948E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.8504541481396948E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.8504541481396948E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4.8504541481396948E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.8504541481396948E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.8504541481396948E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4.8504541481396948E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4.8504541481396948E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4.8504541481396948E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4.8504541481396948E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4.8504541481396948E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4.8504541481396948E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>4.8504541481396948E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>4.8504541481396948E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4.8504541481396948E-2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>4.8504541481396948E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4.8504541481396948E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>4.8504541481396948E-2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>4.8504541481396948E-2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>4.8504541481396948E-2</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4.8504541481396948E-2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>4.8504541481396948E-2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>4.8504541481396948E-2</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>4.8504541481396948E-2</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>4.8504541481396948E-2</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>4.8504541481396948E-2</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>4.8504541481396948E-2</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>4.8504541481396948E-2</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>4.8504541481396948E-2</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>4.8504541481396948E-2</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>4.8504541481396948E-2</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>4.8504541481396948E-2</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>4.8504541481396948E-2</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>4.8504541481396948E-2</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>4.8504541481396948E-2</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>4.8504541481396948E-2</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>4.8504541481396948E-2</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>4.8504541481396948E-2</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>4.8504541481396948E-2</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>4.8504541481396948E-2</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>4.8504541481396948E-2</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>4.8504541481396948E-2</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>4.8504541481396948E-2</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>4.8504541481396948E-2</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>4.8504541481396948E-2</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>4.8504541481396948E-2</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>4.8504541481396948E-2</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>4.8504541481396948E-2</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>4.8504541481396948E-2</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>4.8504541481396948E-2</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>4.8504541481396948E-2</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>4.8504541481396948E-2</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>4.8504541481396948E-2</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>4.8659724597473947E-2</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>4.8659724597473947E-2</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>4.8659724597473947E-2</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>4.8970090829627839E-2</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>4.8970090829627839E-2</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>4.8970090829627839E-2</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>4.8970090829627839E-2</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>5.1022941765160423E-2</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>5.1022941765160423E-2</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>5.1022941765160423E-2</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>5.1022941765160423E-2</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>5.1022941765160423E-2</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>5.5807754510866933E-2</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>5.5807754510866933E-2</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>5.5807754510866933E-2</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>5.8041019014682033E-2</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>5.8041019014682033E-2</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>5.8041019014682033E-2</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>5.727713804329912E-2</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>5.8536338185180808E-2</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>5.8381155069103796E-2</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>5.8381155069103796E-2</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>5.8381155069103796E-2</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>5.8381155069103796E-2</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>5.8381155069103796E-2</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>5.7587504275453019E-2</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>5.7587504275453019E-2</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>5.7587504275453019E-2</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>4.6962543667488782E-2</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>4.711772678356578E-2</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>5.7529103116729763E-2</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>5.7684286232806775E-2</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>5.8788303258611445E-2</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>5.8788303258611445E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-C681-B14E-88EB-832DC22AF12C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1508742544"/>
+        <c:axId val="1508744240"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1508742544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-TW"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1508744240"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1508744240"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-TW"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1508742544"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-TW"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-TW"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-TW"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-TW"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
               <c:f>res!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
@@ -3542,6 +5753,46 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -4097,7 +6348,564 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="圖表 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92C6F4A3-4588-C442-97C0-7D7064491A6A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -4400,11 +7208,1425 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40009FF9-89B2-284C-9AE3-6141A58B2292}">
+  <dimension ref="A1:D100"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O31" sqref="O31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2">
+        <v>0.01</v>
+      </c>
+      <c r="B2">
+        <v>3.6572136990546997E-2</v>
+      </c>
+      <c r="C2">
+        <v>3.6572136990546997E-2</v>
+      </c>
+      <c r="D2">
+        <v>3.6623215394165111E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3">
+        <v>0.02</v>
+      </c>
+      <c r="B3">
+        <v>3.6572136990546997E-2</v>
+      </c>
+      <c r="C3">
+        <v>3.6572136990546997E-2</v>
+      </c>
+      <c r="D3">
+        <v>4.7245341339515273E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
+        <v>0.03</v>
+      </c>
+      <c r="B4">
+        <v>3.6572136990546997E-2</v>
+      </c>
+      <c r="C4">
+        <v>3.6727103672710336E-2</v>
+      </c>
+      <c r="D4">
+        <v>4.7245341339515273E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5">
+        <v>0.04</v>
+      </c>
+      <c r="B5">
+        <v>3.6572136990546997E-2</v>
+      </c>
+      <c r="C5">
+        <v>3.6727103672710336E-2</v>
+      </c>
+      <c r="D5">
+        <v>4.7245341339515273E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
+        <v>0.05</v>
+      </c>
+      <c r="B6">
+        <v>3.6572136990546997E-2</v>
+      </c>
+      <c r="C6">
+        <v>3.7037037037037E-2</v>
+      </c>
+      <c r="D6">
+        <v>4.7245341339515273E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7">
+        <v>0.06</v>
+      </c>
+      <c r="B7">
+        <v>3.6572136990546997E-2</v>
+      </c>
+      <c r="C7">
+        <v>5.7394023921220443E-2</v>
+      </c>
+      <c r="D7">
+        <v>4.7400524455592265E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="B8">
+        <v>4.7192098596760823E-2</v>
+      </c>
+      <c r="C8">
+        <v>6.7753833599176735E-2</v>
+      </c>
+      <c r="D8">
+        <v>4.7400524455592265E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9">
+        <v>0.08</v>
+      </c>
+      <c r="B9">
+        <v>4.7192098596760823E-2</v>
+      </c>
+      <c r="C9">
+        <v>6.5344231070028513E-2</v>
+      </c>
+      <c r="D9">
+        <v>4.7555707571669159E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10">
+        <v>0.09</v>
+      </c>
+      <c r="B10">
+        <v>4.7347065278924155E-2</v>
+      </c>
+      <c r="C10">
+        <v>0.16403752125440027</v>
+      </c>
+      <c r="D10">
+        <v>4.7555707571669159E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11">
+        <v>0.1</v>
+      </c>
+      <c r="B11">
+        <v>4.7347065278924155E-2</v>
+      </c>
+      <c r="C11">
+        <v>0.32895873009570953</v>
+      </c>
+      <c r="D11">
+        <v>4.8504541481396948E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12">
+        <v>0.11</v>
+      </c>
+      <c r="B12">
+        <v>4.7347065278924155E-2</v>
+      </c>
+      <c r="C12">
+        <v>0.3830870177211072</v>
+      </c>
+      <c r="D12">
+        <v>4.8504541481396948E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13">
+        <v>0.12</v>
+      </c>
+      <c r="B13">
+        <v>4.7347065278924155E-2</v>
+      </c>
+      <c r="C13">
+        <v>0.34881156399013036</v>
+      </c>
+      <c r="D13">
+        <v>4.8504541481396948E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14">
+        <v>0.13</v>
+      </c>
+      <c r="B14">
+        <v>4.765699864325082E-2</v>
+      </c>
+      <c r="C14">
+        <v>0.39558102577346793</v>
+      </c>
+      <c r="D14">
+        <v>4.8504541481396948E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="B15">
+        <v>4.7811965325414159E-2</v>
+      </c>
+      <c r="C15">
+        <v>0.50608983329380175</v>
+      </c>
+      <c r="D15">
+        <v>4.8504541481396948E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16">
+        <v>0.15</v>
+      </c>
+      <c r="B16">
+        <v>4.7811965325414159E-2</v>
+      </c>
+      <c r="C16">
+        <v>0.5373553396289581</v>
+      </c>
+      <c r="D16">
+        <v>4.8504541481396948E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17">
+        <v>0.16</v>
+      </c>
+      <c r="B17">
+        <v>5.9062833425809598E-2</v>
+      </c>
+      <c r="C17">
+        <v>0.58127156729278673</v>
+      </c>
+      <c r="D17">
+        <v>4.8504541481396948E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18">
+        <v>0.17</v>
+      </c>
+      <c r="B18">
+        <v>6.0476350948113718E-2</v>
+      </c>
+      <c r="C18">
+        <v>0.66138575374700947</v>
+      </c>
+      <c r="D18">
+        <v>4.8504541481396948E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19">
+        <v>0.18</v>
+      </c>
+      <c r="B19">
+        <v>5.5417367220934648E-2</v>
+      </c>
+      <c r="C19">
+        <v>0.59158112835056398</v>
+      </c>
+      <c r="D19">
+        <v>4.8504541481396948E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20">
+        <v>0.19</v>
+      </c>
+      <c r="B20">
+        <v>5.2666708612535501E-2</v>
+      </c>
+      <c r="C20">
+        <v>0.65535281005058854</v>
+      </c>
+      <c r="D20">
+        <v>4.8504541481396948E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21">
+        <v>0.2</v>
+      </c>
+      <c r="B21">
+        <v>0.10241305262225758</v>
+      </c>
+      <c r="C21">
+        <v>0.64164407837124737</v>
+      </c>
+      <c r="D21">
+        <v>4.8504541481396948E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22">
+        <v>0.21</v>
+      </c>
+      <c r="B22">
+        <v>0.136476842543788</v>
+      </c>
+      <c r="C22">
+        <v>0.64144613001441009</v>
+      </c>
+      <c r="D22">
+        <v>4.8504541481396948E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23">
+        <v>0.22</v>
+      </c>
+      <c r="B23">
+        <v>0.19740058484828349</v>
+      </c>
+      <c r="C23">
+        <v>0.64680549119702069</v>
+      </c>
+      <c r="D23">
+        <v>4.8504541481396948E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24">
+        <v>0.23</v>
+      </c>
+      <c r="B24">
+        <v>0.21175831763480046</v>
+      </c>
+      <c r="C24">
+        <v>0.62922387414536485</v>
+      </c>
+      <c r="D24">
+        <v>4.8504541481396948E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25">
+        <v>0.24</v>
+      </c>
+      <c r="B25">
+        <v>0.19233353100096384</v>
+      </c>
+      <c r="C25">
+        <v>0.6204277110236186</v>
+      </c>
+      <c r="D25">
+        <v>4.8504541481396948E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26">
+        <v>0.25</v>
+      </c>
+      <c r="B26">
+        <v>0.26026173763323857</v>
+      </c>
+      <c r="C26">
+        <v>0.63855246641545493</v>
+      </c>
+      <c r="D26">
+        <v>4.8504541481396948E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27">
+        <v>0.26</v>
+      </c>
+      <c r="B27">
+        <v>0.27004936069079538</v>
+      </c>
+      <c r="C27">
+        <v>0.63518226044537562</v>
+      </c>
+      <c r="D27">
+        <v>4.8504541481396948E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28">
+        <v>0.27</v>
+      </c>
+      <c r="B28">
+        <v>0.25767952870722538</v>
+      </c>
+      <c r="C28">
+        <v>0.61389547346821205</v>
+      </c>
+      <c r="D28">
+        <v>4.8504541481396948E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="B29">
+        <v>0.38817494391526863</v>
+      </c>
+      <c r="C29">
+        <v>0.61300301474442809</v>
+      </c>
+      <c r="D29">
+        <v>4.8504541481396948E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="B30">
+        <v>0.48557450204415947</v>
+      </c>
+      <c r="C30">
+        <v>0.60089482065526278</v>
+      </c>
+      <c r="D30">
+        <v>4.8504541481396948E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31">
+        <v>0.3</v>
+      </c>
+      <c r="B31">
+        <v>0.44132212821878902</v>
+      </c>
+      <c r="C31">
+        <v>0.6154601278773586</v>
+      </c>
+      <c r="D31">
+        <v>4.8504541481396948E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32">
+        <v>0.31</v>
+      </c>
+      <c r="B32">
+        <v>0.43281530847555</v>
+      </c>
+      <c r="C32">
+        <v>0.60796463956345592</v>
+      </c>
+      <c r="D32">
+        <v>4.8504541481396948E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33">
+        <v>0.32</v>
+      </c>
+      <c r="B33">
+        <v>0.43331597371757158</v>
+      </c>
+      <c r="C33">
+        <v>0.58454572179816844</v>
+      </c>
+      <c r="D33">
+        <v>4.8504541481396948E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34">
+        <v>0.33</v>
+      </c>
+      <c r="B34">
+        <v>0.49182648813908819</v>
+      </c>
+      <c r="C34">
+        <v>0.5953468995449529</v>
+      </c>
+      <c r="D34">
+        <v>4.8504541481396948E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35">
+        <v>0.34</v>
+      </c>
+      <c r="B35">
+        <v>0.49094694052225868</v>
+      </c>
+      <c r="C35">
+        <v>0.59178183715636112</v>
+      </c>
+      <c r="D35">
+        <v>4.8504541481396948E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36">
+        <v>0.35</v>
+      </c>
+      <c r="B36">
+        <v>0.49693769953242622</v>
+      </c>
+      <c r="C36">
+        <v>0.57704260813141783</v>
+      </c>
+      <c r="D36">
+        <v>4.8504541481396948E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37">
+        <v>0.36</v>
+      </c>
+      <c r="B37">
+        <v>0.56882727247349874</v>
+      </c>
+      <c r="C37">
+        <v>0.57733969666380036</v>
+      </c>
+      <c r="D37">
+        <v>4.8504541481396948E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38">
+        <v>0.37</v>
+      </c>
+      <c r="B38">
+        <v>0.54167960314830543</v>
+      </c>
+      <c r="C38">
+        <v>0.56209994689421139</v>
+      </c>
+      <c r="D38">
+        <v>4.8504541481396948E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39">
+        <v>0.38</v>
+      </c>
+      <c r="B39">
+        <v>0.58410664654443356</v>
+      </c>
+      <c r="C39">
+        <v>0.56529248656032638</v>
+      </c>
+      <c r="D39">
+        <v>4.8504541481396948E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40">
+        <v>0.39</v>
+      </c>
+      <c r="B40">
+        <v>0.6009564748137397</v>
+      </c>
+      <c r="C40">
+        <v>0.56345509938285465</v>
+      </c>
+      <c r="D40">
+        <v>4.8504541481396948E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41">
+        <v>0.4</v>
+      </c>
+      <c r="B41">
+        <v>0.59916752120347194</v>
+      </c>
+      <c r="C41">
+        <v>0.56156514980856342</v>
+      </c>
+      <c r="D41">
+        <v>4.8504541481396948E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42">
+        <v>0.41</v>
+      </c>
+      <c r="B42">
+        <v>0.6161743239245604</v>
+      </c>
+      <c r="C42">
+        <v>0.48782727214192723</v>
+      </c>
+      <c r="D42">
+        <v>4.8504541481396948E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43">
+        <v>0.42</v>
+      </c>
+      <c r="B43">
+        <v>0.60797963190633886</v>
+      </c>
+      <c r="C43">
+        <v>0.48289400097816326</v>
+      </c>
+      <c r="D43">
+        <v>4.8504541481396948E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44">
+        <v>0.43</v>
+      </c>
+      <c r="B44">
+        <v>0.60252292247359451</v>
+      </c>
+      <c r="C44">
+        <v>0.48289400097816326</v>
+      </c>
+      <c r="D44">
+        <v>4.8504541481396948E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45">
+        <v>0.44</v>
+      </c>
+      <c r="B45">
+        <v>0.59268094667808768</v>
+      </c>
+      <c r="C45">
+        <v>0.47319227106062189</v>
+      </c>
+      <c r="D45">
+        <v>4.8504541481396948E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46">
+        <v>0.45</v>
+      </c>
+      <c r="B46">
+        <v>0.56887347269240196</v>
+      </c>
+      <c r="C46">
+        <v>0.47761299051539052</v>
+      </c>
+      <c r="D46">
+        <v>4.8504541481396948E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47">
+        <v>0.46</v>
+      </c>
+      <c r="B47">
+        <v>0.56647695853118185</v>
+      </c>
+      <c r="C47">
+        <v>0.54561929469190751</v>
+      </c>
+      <c r="D47">
+        <v>4.8504541481396948E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48">
+        <v>0.47</v>
+      </c>
+      <c r="B48">
+        <v>0.56205502514877514</v>
+      </c>
+      <c r="C48">
+        <v>0.54121753398762573</v>
+      </c>
+      <c r="D48">
+        <v>4.8504541481396948E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49">
+        <v>0.48</v>
+      </c>
+      <c r="B49">
+        <v>0.53958087630401774</v>
+      </c>
+      <c r="C49">
+        <v>0.47690586554514841</v>
+      </c>
+      <c r="D49">
+        <v>4.8504541481396948E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50">
+        <v>0.49</v>
+      </c>
+      <c r="B50">
+        <v>0.53705276072912522</v>
+      </c>
+      <c r="C50">
+        <v>0.47690586554514841</v>
+      </c>
+      <c r="D50">
+        <v>4.8504541481396948E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51">
+        <v>0.5</v>
+      </c>
+      <c r="B51">
+        <v>0.52392673211542806</v>
+      </c>
+      <c r="C51">
+        <v>0.47690586554514841</v>
+      </c>
+      <c r="D51">
+        <v>4.8504541481396948E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52">
+        <v>0.51</v>
+      </c>
+      <c r="B52">
+        <v>0.54912958719901139</v>
+      </c>
+      <c r="C52">
+        <v>0.4278396242205118</v>
+      </c>
+      <c r="D52">
+        <v>4.8504541481396948E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53">
+        <v>0.52</v>
+      </c>
+      <c r="B53">
+        <v>0.52725918579099806</v>
+      </c>
+      <c r="C53">
+        <v>0.42976083766564521</v>
+      </c>
+      <c r="D53">
+        <v>4.8504541481396948E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54">
+        <v>0.53</v>
+      </c>
+      <c r="B54">
+        <v>0.44705063588571803</v>
+      </c>
+      <c r="C54">
+        <v>0.42976083766564521</v>
+      </c>
+      <c r="D54">
+        <v>4.8504541481396948E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55">
+        <v>0.54</v>
+      </c>
+      <c r="B55">
+        <v>0.44027491390555074</v>
+      </c>
+      <c r="C55">
+        <v>0.36172096015933053</v>
+      </c>
+      <c r="D55">
+        <v>4.8504541481396948E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="B56">
+        <v>0.42524174014221838</v>
+      </c>
+      <c r="C56">
+        <v>0.35795881721283523</v>
+      </c>
+      <c r="D56">
+        <v>4.8504541481396948E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="B57">
+        <v>0.42306953169497646</v>
+      </c>
+      <c r="C57">
+        <v>0.357076378036562</v>
+      </c>
+      <c r="D57">
+        <v>4.8504541481396948E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="B58">
+        <v>0.42193574484690388</v>
+      </c>
+      <c r="C58">
+        <v>0.42700051904504033</v>
+      </c>
+      <c r="D58">
+        <v>4.8504541481396948E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="B59">
+        <v>0.37830959873628572</v>
+      </c>
+      <c r="C59">
+        <v>0.36941871791762826</v>
+      </c>
+      <c r="D59">
+        <v>4.8504541481396948E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60">
+        <v>0.59</v>
+      </c>
+      <c r="B60">
+        <v>0.45219625041865069</v>
+      </c>
+      <c r="C60">
+        <v>0.36941871791762826</v>
+      </c>
+      <c r="D60">
+        <v>4.8504541481396948E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61">
+        <v>0.6</v>
+      </c>
+      <c r="B61">
+        <v>0.44535956082089762</v>
+      </c>
+      <c r="C61">
+        <v>0.29681720073779777</v>
+      </c>
+      <c r="D61">
+        <v>4.8504541481396948E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62">
+        <v>0.61</v>
+      </c>
+      <c r="B62">
+        <v>0.44117002492423446</v>
+      </c>
+      <c r="C62">
+        <v>0.29340811927738053</v>
+      </c>
+      <c r="D62">
+        <v>4.8504541481396948E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63">
+        <v>0.62</v>
+      </c>
+      <c r="B63">
+        <v>0.43165324177962883</v>
+      </c>
+      <c r="C63">
+        <v>0.28959438261922277</v>
+      </c>
+      <c r="D63">
+        <v>4.8504541481396948E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64">
+        <v>0.63</v>
+      </c>
+      <c r="B64">
+        <v>0.36088406782002624</v>
+      </c>
+      <c r="C64">
+        <v>0.28959438261922277</v>
+      </c>
+      <c r="D64">
+        <v>4.8504541481396948E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65">
+        <v>0.64</v>
+      </c>
+      <c r="B65">
+        <v>0.29007392558131267</v>
+      </c>
+      <c r="C65">
+        <v>0.28959438261922277</v>
+      </c>
+      <c r="D65">
+        <v>4.8504541481396948E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66">
+        <v>0.65</v>
+      </c>
+      <c r="B66">
+        <v>0.27069363867991125</v>
+      </c>
+      <c r="C66">
+        <v>0.28959438261922277</v>
+      </c>
+      <c r="D66">
+        <v>4.8504541481396948E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67">
+        <v>0.66</v>
+      </c>
+      <c r="B67">
+        <v>0.27069363867991125</v>
+      </c>
+      <c r="C67">
+        <v>0.28959438261922277</v>
+      </c>
+      <c r="D67">
+        <v>4.8659724597473947E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68">
+        <v>0.67</v>
+      </c>
+      <c r="B68">
+        <v>0.26932189656742828</v>
+      </c>
+      <c r="C68">
+        <v>0.28614372699465407</v>
+      </c>
+      <c r="D68">
+        <v>4.8659724597473947E-2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69">
+        <v>0.68</v>
+      </c>
+      <c r="B69">
+        <v>0.26273821379769696</v>
+      </c>
+      <c r="C69">
+        <v>0.28683385811956774</v>
+      </c>
+      <c r="D69">
+        <v>4.8659724597473947E-2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70">
+        <v>0.69</v>
+      </c>
+      <c r="B70">
+        <v>0.26136647168521421</v>
+      </c>
+      <c r="C70">
+        <v>0.28683385811956774</v>
+      </c>
+      <c r="D70">
+        <v>4.8970090829627839E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71">
+        <v>0.7</v>
+      </c>
+      <c r="B71">
+        <v>0.25147366825458356</v>
+      </c>
+      <c r="C71">
+        <v>0.28614372699465407</v>
+      </c>
+      <c r="D71">
+        <v>4.8970090829627839E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72">
+        <v>0.71</v>
+      </c>
+      <c r="B72">
+        <v>0.17957494222442316</v>
+      </c>
+      <c r="C72">
+        <v>0.28614372699465407</v>
+      </c>
+      <c r="D72">
+        <v>4.8970090829627839E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73">
+        <v>0.72</v>
+      </c>
+      <c r="B73">
+        <v>0.17758333338328691</v>
+      </c>
+      <c r="C73">
+        <v>0.2845940601730208</v>
+      </c>
+      <c r="D73">
+        <v>4.8970090829627839E-2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74">
+        <v>0.73</v>
+      </c>
+      <c r="B74">
+        <v>0.17758333338328691</v>
+      </c>
+      <c r="C74">
+        <v>0.2845940601730208</v>
+      </c>
+      <c r="D74">
+        <v>5.1022941765160423E-2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75">
+        <v>0.74</v>
+      </c>
+      <c r="B75">
+        <v>0.17758333338328691</v>
+      </c>
+      <c r="C75">
+        <v>0.2845940601730208</v>
+      </c>
+      <c r="D75">
+        <v>5.1022941765160423E-2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76">
+        <v>0.75</v>
+      </c>
+      <c r="B76">
+        <v>0.17419702440268059</v>
+      </c>
+      <c r="C76">
+        <v>0.2845940601730208</v>
+      </c>
+      <c r="D76">
+        <v>5.1022941765160423E-2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77">
+        <v>0.76</v>
+      </c>
+      <c r="B77">
+        <v>0.17419702440268059</v>
+      </c>
+      <c r="C77">
+        <v>0.28276756856130136</v>
+      </c>
+      <c r="D77">
+        <v>5.1022941765160423E-2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78">
+        <v>0.77</v>
+      </c>
+      <c r="B78">
+        <v>0.17419702440268059</v>
+      </c>
+      <c r="C78">
+        <v>0.14656725535534879</v>
+      </c>
+      <c r="D78">
+        <v>5.1022941765160423E-2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79">
+        <v>0.78</v>
+      </c>
+      <c r="B79">
+        <v>0.17357715767402729</v>
+      </c>
+      <c r="C79">
+        <v>0.14656725535534879</v>
+      </c>
+      <c r="D79">
+        <v>5.5807754510866933E-2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80">
+        <v>0.79</v>
+      </c>
+      <c r="B80">
+        <v>0.17130958397788212</v>
+      </c>
+      <c r="C80">
+        <v>0.14656725535534879</v>
+      </c>
+      <c r="D80">
+        <v>5.5807754510866933E-2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81">
+        <v>0.8</v>
+      </c>
+      <c r="B81">
+        <v>0.17130958397788212</v>
+      </c>
+      <c r="C81">
+        <v>0.14612102599345678</v>
+      </c>
+      <c r="D81">
+        <v>5.5807754510866933E-2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="A82">
+        <v>0.81</v>
+      </c>
+      <c r="B82">
+        <v>8.6974501734850218E-2</v>
+      </c>
+      <c r="C82">
+        <v>0.14612102599345678</v>
+      </c>
+      <c r="D82">
+        <v>5.8041019014682033E-2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="A83">
+        <v>0.82</v>
+      </c>
+      <c r="B83">
+        <v>7.3257080610021771E-2</v>
+      </c>
+      <c r="C83">
+        <v>0.14567479663156477</v>
+      </c>
+      <c r="D83">
+        <v>5.8041019014682033E-2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="A84">
+        <v>0.83</v>
+      </c>
+      <c r="B84">
+        <v>7.3257080610021771E-2</v>
+      </c>
+      <c r="C84">
+        <v>0.27981025968466283</v>
+      </c>
+      <c r="D84">
+        <v>5.8041019014682033E-2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="A85">
+        <v>0.84</v>
+      </c>
+      <c r="B85">
+        <v>7.3257080610021771E-2</v>
+      </c>
+      <c r="C85">
+        <v>0.27981025968466283</v>
+      </c>
+      <c r="D85">
+        <v>5.727713804329912E-2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
+      <c r="A86">
+        <v>0.85</v>
+      </c>
+      <c r="B86">
+        <v>7.3257080610021771E-2</v>
+      </c>
+      <c r="C86">
+        <v>0.27912012855974921</v>
+      </c>
+      <c r="D86">
+        <v>5.8536338185180808E-2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
+      <c r="A87">
+        <v>0.86</v>
+      </c>
+      <c r="B87">
+        <v>7.3257080610021771E-2</v>
+      </c>
+      <c r="C87">
+        <v>0.27887622679672741</v>
+      </c>
+      <c r="D87">
+        <v>5.8381155069103796E-2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
+      <c r="A88">
+        <v>0.87</v>
+      </c>
+      <c r="B88">
+        <v>7.3257080610021771E-2</v>
+      </c>
+      <c r="C88">
+        <v>0.25575882791592508</v>
+      </c>
+      <c r="D88">
+        <v>5.8381155069103796E-2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
+      <c r="A89">
+        <v>0.88</v>
+      </c>
+      <c r="B89">
+        <v>7.3257080610021771E-2</v>
+      </c>
+      <c r="C89">
+        <v>0.20133705920844222</v>
+      </c>
+      <c r="D89">
+        <v>5.8381155069103796E-2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
+      <c r="A90">
+        <v>0.89</v>
+      </c>
+      <c r="B90">
+        <v>7.3257080610021771E-2</v>
+      </c>
+      <c r="C90">
+        <v>0.20158096097146397</v>
+      </c>
+      <c r="D90">
+        <v>5.8381155069103796E-2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
+      <c r="A91">
+        <v>0.9</v>
+      </c>
+      <c r="B91">
+        <v>7.3257080610021771E-2</v>
+      </c>
+      <c r="C91">
+        <v>0.13123747522724488</v>
+      </c>
+      <c r="D91">
+        <v>5.8381155069103796E-2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
+      <c r="A92">
+        <v>0.91</v>
+      </c>
+      <c r="B92">
+        <v>7.3257080610021771E-2</v>
+      </c>
+      <c r="C92">
+        <v>0.1969523706959381</v>
+      </c>
+      <c r="D92">
+        <v>5.7587504275453019E-2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
+      <c r="A93">
+        <v>0.92</v>
+      </c>
+      <c r="B93">
+        <v>7.3257080610021771E-2</v>
+      </c>
+      <c r="C93">
+        <v>0.19605991197215411</v>
+      </c>
+      <c r="D93">
+        <v>5.7587504275453019E-2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4">
+      <c r="A94">
+        <v>0.93</v>
+      </c>
+      <c r="B94">
+        <v>7.3257080610021771E-2</v>
+      </c>
+      <c r="C94">
+        <v>0.19605991197215411</v>
+      </c>
+      <c r="D94">
+        <v>5.7587504275453019E-2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4">
+      <c r="A95">
+        <v>0.94</v>
+      </c>
+      <c r="B95">
+        <v>7.3257080610021771E-2</v>
+      </c>
+      <c r="C95">
+        <v>0.19605991197215411</v>
+      </c>
+      <c r="D95">
+        <v>4.6962543667488782E-2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
+      <c r="A96">
+        <v>0.95</v>
+      </c>
+      <c r="B96">
+        <v>7.3257080610021771E-2</v>
+      </c>
+      <c r="C96">
+        <v>0.19605991197215411</v>
+      </c>
+      <c r="D96">
+        <v>4.711772678356578E-2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
+      <c r="A97">
+        <v>0.96</v>
+      </c>
+      <c r="B97">
+        <v>7.3257080610021771E-2</v>
+      </c>
+      <c r="C97">
+        <v>0.19561368261026213</v>
+      </c>
+      <c r="D97">
+        <v>5.7529103116729763E-2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
+      <c r="A98">
+        <v>0.97</v>
+      </c>
+      <c r="B98">
+        <v>7.3257080610021771E-2</v>
+      </c>
+      <c r="C98">
+        <v>0.19561368261026213</v>
+      </c>
+      <c r="D98">
+        <v>5.7684286232806775E-2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4">
+      <c r="A99">
+        <v>0.98</v>
+      </c>
+      <c r="B99">
+        <v>7.3257080610021771E-2</v>
+      </c>
+      <c r="C99">
+        <v>0.19492355148534846</v>
+      </c>
+      <c r="D99">
+        <v>5.8788303258611445E-2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4">
+      <c r="A100">
+        <v>0.99</v>
+      </c>
+      <c r="B100">
+        <v>7.3257080610021771E-2</v>
+      </c>
+      <c r="C100">
+        <v>0.19492355148534846</v>
+      </c>
+      <c r="D100">
+        <v>5.8788303258611445E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AP102"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E100" sqref="A1:E100"/>
+      <selection activeCell="A2" sqref="A2:A100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
@@ -17734,12 +21956,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7874504A-2638-A74A-B28E-EB1F3DEA8608}">
-  <dimension ref="A1:AP100"/>
+  <dimension ref="A1:AP101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F100"/>
+    <sheetView topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -31034,18 +35256,25 @@
         <v>0</v>
       </c>
     </row>
+    <row r="101" spans="1:42">
+      <c r="B101" s="2">
+        <f>MAX(B2:B100)</f>
+        <v>0.6161743239245604</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ED48E34-ED81-AD40-8188-BF620A178A69}">
   <dimension ref="A1:AP100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F100"/>
+      <selection activeCell="B2" sqref="B2:B100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -44346,12 +48575,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98396959-F581-9D41-88CF-A7D05F17DAF2}">
   <dimension ref="A1:AP100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F100"/>
+      <selection activeCell="D81" sqref="D81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>